<commit_message>
Dictame de aceptacion 1.2
</commit_message>
<xml_diff>
--- a/TT1/Product Backlog.xlsx
+++ b/TT1/Product Backlog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Downloads\Trabajo Terminal\TT1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{603D82A2-B910-469F-9988-DA74494CBDC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{610BDD74-3CCA-44A7-940C-803D0C810FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,12 +16,12 @@
     <sheet name="Agile Product Backlog" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Agile Product Backlog'!$B$1:$M$27</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Agile Product Backlog'!$B$1:$N$27</definedName>
     <definedName name="Priority">'Agile Product Backlog'!#REF!</definedName>
     <definedName name="Status">'Agile Product Backlog'!#REF!</definedName>
     <definedName name="YesNo">'Agile Product Backlog'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>Sprint 3</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t>To DO</t>
+  </si>
+  <si>
+    <t>Criterios de aceptacion</t>
   </si>
 </sst>
 </file>
@@ -637,32 +640,32 @@
     <tabColor theme="0" tint="-4.9989318521683403E-2"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AI66"/>
+  <dimension ref="B1:AJ66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O4" sqref="O4"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="3.296875" style="3" customWidth="1"/>
     <col min="2" max="2" width="10.796875" style="3" customWidth="1"/>
-    <col min="3" max="5" width="33.19921875" style="3" customWidth="1"/>
-    <col min="6" max="7" width="11.296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.796875" style="3" customWidth="1"/>
-    <col min="10" max="10" width="9.59765625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.09765625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.796875" style="3" customWidth="1"/>
-    <col min="13" max="13" width="10.796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="3.296875" style="3" customWidth="1"/>
-    <col min="15" max="17" width="17.796875" style="3" customWidth="1"/>
-    <col min="18" max="18" width="3.296875" style="3" customWidth="1"/>
-    <col min="19" max="16384" width="10.796875" style="3"/>
+    <col min="3" max="6" width="33.19921875" style="3" customWidth="1"/>
+    <col min="7" max="8" width="11.296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.796875" style="3" customWidth="1"/>
+    <col min="11" max="11" width="9.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.09765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.796875" style="3" customWidth="1"/>
+    <col min="14" max="14" width="10.796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.296875" style="3" customWidth="1"/>
+    <col min="16" max="18" width="17.796875" style="3" customWidth="1"/>
+    <col min="19" max="19" width="3.296875" style="3" customWidth="1"/>
+    <col min="20" max="16384" width="10.796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:35" ht="34.950000000000003" customHeight="1">
+    <row r="1" spans="2:36" ht="34.950000000000003" customHeight="1">
       <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
@@ -670,36 +673,38 @@
         <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="2"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
@@ -721,45 +726,46 @@
       <c r="AG1" s="2"/>
       <c r="AH1" s="2"/>
       <c r="AI1" s="2"/>
-    </row>
-    <row r="2" spans="2:35" ht="39.6">
+      <c r="AJ1" s="2"/>
+    </row>
+    <row r="2" spans="2:36" ht="39.6">
       <c r="B2" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="6"/>
+      <c r="E2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="7">
+      <c r="G2" s="7">
         <v>45916</v>
       </c>
-      <c r="G2" s="7">
+      <c r="H2" s="7">
         <v>45923</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>3</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>3</v>
       </c>
       <c r="J2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="6">
+      <c r="M2" s="6">
         <v>10</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
@@ -778,45 +784,46 @@
       <c r="AD2" s="2"/>
       <c r="AE2" s="2"/>
       <c r="AF2" s="2"/>
-    </row>
-    <row r="3" spans="2:35" ht="34.950000000000003" customHeight="1">
+      <c r="AG2" s="2"/>
+    </row>
+    <row r="3" spans="2:36" ht="34.950000000000003" customHeight="1">
       <c r="B3" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="6"/>
+      <c r="E3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="7">
+      <c r="G3" s="7">
         <v>45924</v>
       </c>
-      <c r="G3" s="7">
+      <c r="H3" s="7">
         <v>45930</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>3</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>3</v>
       </c>
       <c r="J3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="L3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="6">
+      <c r="M3" s="6">
         <v>8</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="N3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
@@ -835,21 +842,22 @@
       <c r="AD3" s="2"/>
       <c r="AE3" s="2"/>
       <c r="AF3" s="2"/>
-    </row>
-    <row r="4" spans="2:35" ht="34.950000000000003" customHeight="1">
+      <c r="AG3" s="2"/>
+    </row>
+    <row r="4" spans="2:36" ht="34.950000000000003" customHeight="1">
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
-      <c r="F4" s="5"/>
+      <c r="F4" s="4"/>
       <c r="G4" s="5"/>
-      <c r="H4" s="4"/>
+      <c r="H4" s="5"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
-      <c r="N4" s="2"/>
+      <c r="N4" s="4"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
@@ -868,45 +876,46 @@
       <c r="AD4" s="2"/>
       <c r="AE4" s="2"/>
       <c r="AF4" s="2"/>
-    </row>
-    <row r="5" spans="2:35" ht="34.950000000000003" customHeight="1">
+      <c r="AG4" s="2"/>
+    </row>
+    <row r="5" spans="2:36" ht="34.950000000000003" customHeight="1">
       <c r="B5" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="6"/>
+      <c r="E5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="7">
+      <c r="G5" s="7">
         <v>45931</v>
       </c>
-      <c r="G5" s="7">
+      <c r="H5" s="7">
         <v>45945</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="I5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="J5" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="K5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="L5" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="L5" s="6">
+      <c r="M5" s="6">
         <v>4</v>
       </c>
-      <c r="M5" s="6" t="s">
+      <c r="N5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
@@ -925,21 +934,22 @@
       <c r="AD5" s="2"/>
       <c r="AE5" s="2"/>
       <c r="AF5" s="2"/>
-    </row>
-    <row r="6" spans="2:35" ht="34.950000000000003" customHeight="1">
+      <c r="AG5" s="2"/>
+    </row>
+    <row r="6" spans="2:36" ht="34.950000000000003" customHeight="1">
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
-      <c r="F6" s="7"/>
+      <c r="F6" s="6"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="6"/>
+      <c r="H6" s="7"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
-      <c r="N6" s="2"/>
+      <c r="N6" s="6"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
@@ -961,21 +971,22 @@
       <c r="AG6" s="2"/>
       <c r="AH6" s="2"/>
       <c r="AI6" s="2"/>
-    </row>
-    <row r="7" spans="2:35" ht="34.950000000000003" customHeight="1">
+      <c r="AJ6" s="2"/>
+    </row>
+    <row r="7" spans="2:36" ht="34.950000000000003" customHeight="1">
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
-      <c r="F7" s="7"/>
+      <c r="F7" s="6"/>
       <c r="G7" s="7"/>
-      <c r="H7" s="6"/>
+      <c r="H7" s="7"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
-      <c r="N7" s="2"/>
+      <c r="N7" s="6"/>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
@@ -997,23 +1008,24 @@
       <c r="AG7" s="2"/>
       <c r="AH7" s="2"/>
       <c r="AI7" s="2"/>
-    </row>
-    <row r="8" spans="2:35" ht="34.950000000000003" customHeight="1">
+      <c r="AJ7" s="2"/>
+    </row>
+    <row r="8" spans="2:36" ht="34.950000000000003" customHeight="1">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="4"/>
+      <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="5"/>
+      <c r="F8" s="4"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="4"/>
+      <c r="H8" s="5"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
-      <c r="N8" s="2"/>
+      <c r="N8" s="4"/>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
@@ -1035,21 +1047,22 @@
       <c r="AG8" s="2"/>
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
-    </row>
-    <row r="9" spans="2:35" ht="34.950000000000003" customHeight="1">
+      <c r="AJ8" s="2"/>
+    </row>
+    <row r="9" spans="2:36" ht="34.950000000000003" customHeight="1">
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
-      <c r="F9" s="7"/>
+      <c r="F9" s="6"/>
       <c r="G9" s="7"/>
-      <c r="H9" s="6"/>
+      <c r="H9" s="7"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
-      <c r="N9" s="2"/>
+      <c r="N9" s="6"/>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
@@ -1071,21 +1084,22 @@
       <c r="AG9" s="2"/>
       <c r="AH9" s="2"/>
       <c r="AI9" s="2"/>
-    </row>
-    <row r="10" spans="2:35" ht="34.950000000000003" customHeight="1">
+      <c r="AJ9" s="2"/>
+    </row>
+    <row r="10" spans="2:36" ht="34.950000000000003" customHeight="1">
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
-      <c r="F10" s="7"/>
+      <c r="F10" s="6"/>
       <c r="G10" s="7"/>
-      <c r="H10" s="6"/>
+      <c r="H10" s="7"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
-      <c r="N10" s="2"/>
+      <c r="N10" s="6"/>
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
@@ -1107,21 +1121,22 @@
       <c r="AG10" s="2"/>
       <c r="AH10" s="2"/>
       <c r="AI10" s="2"/>
-    </row>
-    <row r="11" spans="2:35" ht="34.950000000000003" customHeight="1">
+      <c r="AJ10" s="2"/>
+    </row>
+    <row r="11" spans="2:36" ht="34.950000000000003" customHeight="1">
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
-      <c r="F11" s="7"/>
+      <c r="F11" s="6"/>
       <c r="G11" s="7"/>
-      <c r="H11" s="6"/>
+      <c r="H11" s="7"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
-      <c r="N11" s="2"/>
+      <c r="N11" s="6"/>
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
@@ -1143,23 +1158,24 @@
       <c r="AG11" s="2"/>
       <c r="AH11" s="2"/>
       <c r="AI11" s="2"/>
-    </row>
-    <row r="12" spans="2:35" ht="34.950000000000003" customHeight="1">
+      <c r="AJ11" s="2"/>
+    </row>
+    <row r="12" spans="2:36" ht="34.950000000000003" customHeight="1">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="4"/>
+      <c r="E12" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="5"/>
+      <c r="F12" s="4"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="4"/>
+      <c r="H12" s="5"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
-      <c r="N12" s="2"/>
+      <c r="N12" s="4"/>
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
@@ -1181,21 +1197,22 @@
       <c r="AG12" s="2"/>
       <c r="AH12" s="2"/>
       <c r="AI12" s="2"/>
-    </row>
-    <row r="13" spans="2:35" ht="34.950000000000003" customHeight="1">
+      <c r="AJ12" s="2"/>
+    </row>
+    <row r="13" spans="2:36" ht="34.950000000000003" customHeight="1">
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="7"/>
+      <c r="F13" s="6"/>
       <c r="G13" s="7"/>
-      <c r="H13" s="6"/>
+      <c r="H13" s="7"/>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
-      <c r="N13" s="2"/>
+      <c r="N13" s="6"/>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
@@ -1217,21 +1234,22 @@
       <c r="AG13" s="2"/>
       <c r="AH13" s="2"/>
       <c r="AI13" s="2"/>
-    </row>
-    <row r="14" spans="2:35" ht="34.950000000000003" customHeight="1">
+      <c r="AJ13" s="2"/>
+    </row>
+    <row r="14" spans="2:36" ht="34.950000000000003" customHeight="1">
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="7"/>
+      <c r="F14" s="6"/>
       <c r="G14" s="7"/>
-      <c r="H14" s="6"/>
+      <c r="H14" s="7"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
-      <c r="N14" s="2"/>
+      <c r="N14" s="6"/>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
@@ -1253,21 +1271,22 @@
       <c r="AG14" s="2"/>
       <c r="AH14" s="2"/>
       <c r="AI14" s="2"/>
-    </row>
-    <row r="15" spans="2:35" ht="34.950000000000003" customHeight="1">
+      <c r="AJ14" s="2"/>
+    </row>
+    <row r="15" spans="2:36" ht="34.950000000000003" customHeight="1">
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="7"/>
+      <c r="F15" s="6"/>
       <c r="G15" s="7"/>
-      <c r="H15" s="6"/>
+      <c r="H15" s="7"/>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
-      <c r="N15" s="2"/>
+      <c r="N15" s="6"/>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
@@ -1289,23 +1308,24 @@
       <c r="AG15" s="2"/>
       <c r="AH15" s="2"/>
       <c r="AI15" s="2"/>
-    </row>
-    <row r="16" spans="2:35" ht="34.950000000000003" customHeight="1">
+      <c r="AJ15" s="2"/>
+    </row>
+    <row r="16" spans="2:36" ht="34.950000000000003" customHeight="1">
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="4"/>
+      <c r="E16" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="5"/>
+      <c r="F16" s="4"/>
       <c r="G16" s="5"/>
-      <c r="H16" s="4"/>
+      <c r="H16" s="5"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
-      <c r="N16" s="2"/>
+      <c r="N16" s="4"/>
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
@@ -1327,21 +1347,22 @@
       <c r="AG16" s="2"/>
       <c r="AH16" s="2"/>
       <c r="AI16" s="2"/>
-    </row>
-    <row r="17" spans="2:35" ht="34.950000000000003" customHeight="1">
+      <c r="AJ16" s="2"/>
+    </row>
+    <row r="17" spans="2:36" ht="34.950000000000003" customHeight="1">
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
-      <c r="F17" s="7"/>
+      <c r="F17" s="6"/>
       <c r="G17" s="7"/>
-      <c r="H17" s="6"/>
+      <c r="H17" s="7"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
-      <c r="N17" s="2"/>
+      <c r="N17" s="6"/>
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
@@ -1363,21 +1384,22 @@
       <c r="AG17" s="2"/>
       <c r="AH17" s="2"/>
       <c r="AI17" s="2"/>
-    </row>
-    <row r="18" spans="2:35" ht="34.950000000000003" customHeight="1">
+      <c r="AJ17" s="2"/>
+    </row>
+    <row r="18" spans="2:36" ht="34.950000000000003" customHeight="1">
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
-      <c r="F18" s="7"/>
+      <c r="F18" s="6"/>
       <c r="G18" s="7"/>
-      <c r="H18" s="6"/>
+      <c r="H18" s="7"/>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
-      <c r="N18" s="2"/>
+      <c r="N18" s="6"/>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
@@ -1399,21 +1421,22 @@
       <c r="AG18" s="2"/>
       <c r="AH18" s="2"/>
       <c r="AI18" s="2"/>
-    </row>
-    <row r="19" spans="2:35" ht="34.950000000000003" customHeight="1">
+      <c r="AJ18" s="2"/>
+    </row>
+    <row r="19" spans="2:36" ht="34.950000000000003" customHeight="1">
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
-      <c r="F19" s="7"/>
+      <c r="F19" s="6"/>
       <c r="G19" s="7"/>
-      <c r="H19" s="6"/>
+      <c r="H19" s="7"/>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
-      <c r="N19" s="2"/>
+      <c r="N19" s="6"/>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
@@ -1435,23 +1458,24 @@
       <c r="AG19" s="2"/>
       <c r="AH19" s="2"/>
       <c r="AI19" s="2"/>
-    </row>
-    <row r="20" spans="2:35" ht="34.950000000000003" customHeight="1">
+      <c r="AJ19" s="2"/>
+    </row>
+    <row r="20" spans="2:36" ht="34.950000000000003" customHeight="1">
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="4"/>
+      <c r="E20" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="5"/>
+      <c r="F20" s="4"/>
       <c r="G20" s="5"/>
-      <c r="H20" s="4"/>
+      <c r="H20" s="5"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
-      <c r="N20" s="2"/>
+      <c r="N20" s="4"/>
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
@@ -1473,21 +1497,22 @@
       <c r="AG20" s="2"/>
       <c r="AH20" s="2"/>
       <c r="AI20" s="2"/>
-    </row>
-    <row r="21" spans="2:35" ht="34.950000000000003" customHeight="1">
+      <c r="AJ20" s="2"/>
+    </row>
+    <row r="21" spans="2:36" ht="34.950000000000003" customHeight="1">
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
-      <c r="F21" s="7"/>
+      <c r="F21" s="6"/>
       <c r="G21" s="7"/>
-      <c r="H21" s="6"/>
+      <c r="H21" s="7"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
-      <c r="N21" s="2"/>
+      <c r="N21" s="6"/>
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
@@ -1509,21 +1534,22 @@
       <c r="AG21" s="2"/>
       <c r="AH21" s="2"/>
       <c r="AI21" s="2"/>
-    </row>
-    <row r="22" spans="2:35" ht="34.950000000000003" customHeight="1">
+      <c r="AJ21" s="2"/>
+    </row>
+    <row r="22" spans="2:36" ht="34.950000000000003" customHeight="1">
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
-      <c r="F22" s="7"/>
+      <c r="F22" s="6"/>
       <c r="G22" s="7"/>
-      <c r="H22" s="6"/>
+      <c r="H22" s="7"/>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
-      <c r="N22" s="2"/>
+      <c r="N22" s="6"/>
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
@@ -1545,21 +1571,22 @@
       <c r="AG22" s="2"/>
       <c r="AH22" s="2"/>
       <c r="AI22" s="2"/>
-    </row>
-    <row r="23" spans="2:35" ht="34.950000000000003" customHeight="1">
+      <c r="AJ22" s="2"/>
+    </row>
+    <row r="23" spans="2:36" ht="34.950000000000003" customHeight="1">
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
-      <c r="F23" s="7"/>
+      <c r="F23" s="6"/>
       <c r="G23" s="7"/>
-      <c r="H23" s="6"/>
+      <c r="H23" s="7"/>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
-      <c r="N23" s="2"/>
+      <c r="N23" s="6"/>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
@@ -1581,23 +1608,24 @@
       <c r="AG23" s="2"/>
       <c r="AH23" s="2"/>
       <c r="AI23" s="2"/>
-    </row>
-    <row r="24" spans="2:35" ht="34.950000000000003" customHeight="1">
+      <c r="AJ23" s="2"/>
+    </row>
+    <row r="24" spans="2:36" ht="34.950000000000003" customHeight="1">
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="4"/>
+      <c r="E24" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E24" s="4"/>
-      <c r="F24" s="5"/>
+      <c r="F24" s="4"/>
       <c r="G24" s="5"/>
-      <c r="H24" s="4"/>
+      <c r="H24" s="5"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
-      <c r="N24" s="2"/>
+      <c r="N24" s="4"/>
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
@@ -1619,21 +1647,22 @@
       <c r="AG24" s="2"/>
       <c r="AH24" s="2"/>
       <c r="AI24" s="2"/>
-    </row>
-    <row r="25" spans="2:35" ht="34.950000000000003" customHeight="1">
+      <c r="AJ24" s="2"/>
+    </row>
+    <row r="25" spans="2:36" ht="34.950000000000003" customHeight="1">
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
-      <c r="F25" s="7"/>
+      <c r="F25" s="6"/>
       <c r="G25" s="7"/>
-      <c r="H25" s="6"/>
+      <c r="H25" s="7"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
-      <c r="N25" s="2"/>
+      <c r="N25" s="6"/>
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
@@ -1655,21 +1684,22 @@
       <c r="AG25" s="2"/>
       <c r="AH25" s="2"/>
       <c r="AI25" s="2"/>
-    </row>
-    <row r="26" spans="2:35" ht="34.950000000000003" customHeight="1">
+      <c r="AJ25" s="2"/>
+    </row>
+    <row r="26" spans="2:36" ht="34.950000000000003" customHeight="1">
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
-      <c r="F26" s="7"/>
+      <c r="F26" s="6"/>
       <c r="G26" s="7"/>
-      <c r="H26" s="6"/>
+      <c r="H26" s="7"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
-      <c r="N26" s="2"/>
+      <c r="N26" s="6"/>
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
@@ -1691,21 +1721,22 @@
       <c r="AG26" s="2"/>
       <c r="AH26" s="2"/>
       <c r="AI26" s="2"/>
-    </row>
-    <row r="27" spans="2:35" ht="34.950000000000003" customHeight="1">
+      <c r="AJ26" s="2"/>
+    </row>
+    <row r="27" spans="2:36" ht="34.950000000000003" customHeight="1">
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
-      <c r="F27" s="7"/>
+      <c r="F27" s="6"/>
       <c r="G27" s="7"/>
-      <c r="H27" s="6"/>
+      <c r="H27" s="7"/>
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
-      <c r="N27" s="2"/>
+      <c r="N27" s="6"/>
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
@@ -1727,8 +1758,9 @@
       <c r="AG27" s="2"/>
       <c r="AH27" s="2"/>
       <c r="AI27" s="2"/>
-    </row>
-    <row r="28" spans="2:35" ht="10.050000000000001" customHeight="1">
+      <c r="AJ27" s="2"/>
+    </row>
+    <row r="28" spans="2:36" ht="10.050000000000001" customHeight="1">
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -1762,8 +1794,9 @@
       <c r="AG28" s="2"/>
       <c r="AH28" s="2"/>
       <c r="AI28" s="2"/>
-    </row>
-    <row r="29" spans="2:35" s="9" customFormat="1" ht="49.95" customHeight="1">
+      <c r="AJ28" s="2"/>
+    </row>
+    <row r="29" spans="2:36" s="9" customFormat="1" ht="49.95" customHeight="1">
       <c r="B29" s="10" t="s">
         <v>16</v>
       </c>
@@ -1778,10 +1811,10 @@
       <c r="K29" s="11"/>
       <c r="L29" s="11"/>
       <c r="M29" s="11"/>
-      <c r="N29"/>
+      <c r="N29" s="11"/>
       <c r="O29"/>
       <c r="P29"/>
-      <c r="Q29" s="8"/>
+      <c r="Q29"/>
       <c r="R29" s="8"/>
       <c r="S29" s="8"/>
       <c r="T29" s="8"/>
@@ -1800,8 +1833,9 @@
       <c r="AG29" s="8"/>
       <c r="AH29" s="8"/>
       <c r="AI29" s="8"/>
-    </row>
-    <row r="30" spans="2:35">
+      <c r="AJ29" s="8"/>
+    </row>
+    <row r="30" spans="2:36">
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1835,8 +1869,9 @@
       <c r="AG30" s="2"/>
       <c r="AH30" s="2"/>
       <c r="AI30" s="2"/>
-    </row>
-    <row r="31" spans="2:35">
+      <c r="AJ30" s="2"/>
+    </row>
+    <row r="31" spans="2:36">
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -1870,8 +1905,9 @@
       <c r="AG31" s="2"/>
       <c r="AH31" s="2"/>
       <c r="AI31" s="2"/>
-    </row>
-    <row r="32" spans="2:35">
+      <c r="AJ31" s="2"/>
+    </row>
+    <row r="32" spans="2:36">
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -1905,8 +1941,9 @@
       <c r="AG32" s="2"/>
       <c r="AH32" s="2"/>
       <c r="AI32" s="2"/>
-    </row>
-    <row r="33" spans="3:35">
+      <c r="AJ32" s="2"/>
+    </row>
+    <row r="33" spans="3:36">
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -1940,8 +1977,9 @@
       <c r="AG33" s="2"/>
       <c r="AH33" s="2"/>
       <c r="AI33" s="2"/>
-    </row>
-    <row r="34" spans="3:35">
+      <c r="AJ33" s="2"/>
+    </row>
+    <row r="34" spans="3:36">
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -1975,8 +2013,9 @@
       <c r="AG34" s="2"/>
       <c r="AH34" s="2"/>
       <c r="AI34" s="2"/>
-    </row>
-    <row r="35" spans="3:35">
+      <c r="AJ34" s="2"/>
+    </row>
+    <row r="35" spans="3:36">
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -2010,8 +2049,9 @@
       <c r="AG35" s="2"/>
       <c r="AH35" s="2"/>
       <c r="AI35" s="2"/>
-    </row>
-    <row r="36" spans="3:35">
+      <c r="AJ35" s="2"/>
+    </row>
+    <row r="36" spans="3:36">
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -2045,8 +2085,9 @@
       <c r="AG36" s="2"/>
       <c r="AH36" s="2"/>
       <c r="AI36" s="2"/>
-    </row>
-    <row r="37" spans="3:35">
+      <c r="AJ36" s="2"/>
+    </row>
+    <row r="37" spans="3:36">
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -2080,8 +2121,9 @@
       <c r="AG37" s="2"/>
       <c r="AH37" s="2"/>
       <c r="AI37" s="2"/>
-    </row>
-    <row r="38" spans="3:35">
+      <c r="AJ37" s="2"/>
+    </row>
+    <row r="38" spans="3:36">
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -2115,8 +2157,9 @@
       <c r="AG38" s="2"/>
       <c r="AH38" s="2"/>
       <c r="AI38" s="2"/>
-    </row>
-    <row r="39" spans="3:35">
+      <c r="AJ38" s="2"/>
+    </row>
+    <row r="39" spans="3:36">
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -2150,8 +2193,9 @@
       <c r="AG39" s="2"/>
       <c r="AH39" s="2"/>
       <c r="AI39" s="2"/>
-    </row>
-    <row r="40" spans="3:35">
+      <c r="AJ39" s="2"/>
+    </row>
+    <row r="40" spans="3:36">
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -2185,8 +2229,9 @@
       <c r="AG40" s="2"/>
       <c r="AH40" s="2"/>
       <c r="AI40" s="2"/>
-    </row>
-    <row r="41" spans="3:35">
+      <c r="AJ40" s="2"/>
+    </row>
+    <row r="41" spans="3:36">
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -2220,8 +2265,9 @@
       <c r="AG41" s="2"/>
       <c r="AH41" s="2"/>
       <c r="AI41" s="2"/>
-    </row>
-    <row r="42" spans="3:35">
+      <c r="AJ41" s="2"/>
+    </row>
+    <row r="42" spans="3:36">
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -2255,8 +2301,9 @@
       <c r="AG42" s="2"/>
       <c r="AH42" s="2"/>
       <c r="AI42" s="2"/>
-    </row>
-    <row r="43" spans="3:35">
+      <c r="AJ42" s="2"/>
+    </row>
+    <row r="43" spans="3:36">
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -2290,8 +2337,9 @@
       <c r="AG43" s="2"/>
       <c r="AH43" s="2"/>
       <c r="AI43" s="2"/>
-    </row>
-    <row r="44" spans="3:35">
+      <c r="AJ43" s="2"/>
+    </row>
+    <row r="44" spans="3:36">
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -2325,8 +2373,9 @@
       <c r="AG44" s="2"/>
       <c r="AH44" s="2"/>
       <c r="AI44" s="2"/>
-    </row>
-    <row r="45" spans="3:35">
+      <c r="AJ44" s="2"/>
+    </row>
+    <row r="45" spans="3:36">
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -2360,8 +2409,9 @@
       <c r="AG45" s="2"/>
       <c r="AH45" s="2"/>
       <c r="AI45" s="2"/>
-    </row>
-    <row r="46" spans="3:35">
+      <c r="AJ45" s="2"/>
+    </row>
+    <row r="46" spans="3:36">
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -2395,8 +2445,9 @@
       <c r="AG46" s="2"/>
       <c r="AH46" s="2"/>
       <c r="AI46" s="2"/>
-    </row>
-    <row r="47" spans="3:35">
+      <c r="AJ46" s="2"/>
+    </row>
+    <row r="47" spans="3:36">
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -2430,8 +2481,9 @@
       <c r="AG47" s="2"/>
       <c r="AH47" s="2"/>
       <c r="AI47" s="2"/>
-    </row>
-    <row r="48" spans="3:35">
+      <c r="AJ47" s="2"/>
+    </row>
+    <row r="48" spans="3:36">
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -2465,8 +2517,9 @@
       <c r="AG48" s="2"/>
       <c r="AH48" s="2"/>
       <c r="AI48" s="2"/>
-    </row>
-    <row r="49" spans="3:35">
+      <c r="AJ48" s="2"/>
+    </row>
+    <row r="49" spans="3:36">
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
@@ -2500,8 +2553,9 @@
       <c r="AG49" s="2"/>
       <c r="AH49" s="2"/>
       <c r="AI49" s="2"/>
-    </row>
-    <row r="50" spans="3:35">
+      <c r="AJ49" s="2"/>
+    </row>
+    <row r="50" spans="3:36">
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -2535,8 +2589,9 @@
       <c r="AG50" s="2"/>
       <c r="AH50" s="2"/>
       <c r="AI50" s="2"/>
-    </row>
-    <row r="51" spans="3:35">
+      <c r="AJ50" s="2"/>
+    </row>
+    <row r="51" spans="3:36">
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -2570,8 +2625,9 @@
       <c r="AG51" s="2"/>
       <c r="AH51" s="2"/>
       <c r="AI51" s="2"/>
-    </row>
-    <row r="52" spans="3:35">
+      <c r="AJ51" s="2"/>
+    </row>
+    <row r="52" spans="3:36">
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
@@ -2605,8 +2661,9 @@
       <c r="AG52" s="2"/>
       <c r="AH52" s="2"/>
       <c r="AI52" s="2"/>
-    </row>
-    <row r="53" spans="3:35">
+      <c r="AJ52" s="2"/>
+    </row>
+    <row r="53" spans="3:36">
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
@@ -2640,8 +2697,9 @@
       <c r="AG53" s="2"/>
       <c r="AH53" s="2"/>
       <c r="AI53" s="2"/>
-    </row>
-    <row r="54" spans="3:35">
+      <c r="AJ53" s="2"/>
+    </row>
+    <row r="54" spans="3:36">
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
@@ -2675,8 +2733,9 @@
       <c r="AG54" s="2"/>
       <c r="AH54" s="2"/>
       <c r="AI54" s="2"/>
-    </row>
-    <row r="55" spans="3:35">
+      <c r="AJ54" s="2"/>
+    </row>
+    <row r="55" spans="3:36">
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -2710,8 +2769,9 @@
       <c r="AG55" s="2"/>
       <c r="AH55" s="2"/>
       <c r="AI55" s="2"/>
-    </row>
-    <row r="56" spans="3:35">
+      <c r="AJ55" s="2"/>
+    </row>
+    <row r="56" spans="3:36">
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -2745,8 +2805,9 @@
       <c r="AG56" s="2"/>
       <c r="AH56" s="2"/>
       <c r="AI56" s="2"/>
-    </row>
-    <row r="57" spans="3:35">
+      <c r="AJ56" s="2"/>
+    </row>
+    <row r="57" spans="3:36">
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
@@ -2780,8 +2841,9 @@
       <c r="AG57" s="2"/>
       <c r="AH57" s="2"/>
       <c r="AI57" s="2"/>
-    </row>
-    <row r="58" spans="3:35">
+      <c r="AJ57" s="2"/>
+    </row>
+    <row r="58" spans="3:36">
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
@@ -2815,8 +2877,9 @@
       <c r="AG58" s="2"/>
       <c r="AH58" s="2"/>
       <c r="AI58" s="2"/>
-    </row>
-    <row r="59" spans="3:35">
+      <c r="AJ58" s="2"/>
+    </row>
+    <row r="59" spans="3:36">
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
@@ -2850,8 +2913,9 @@
       <c r="AG59" s="2"/>
       <c r="AH59" s="2"/>
       <c r="AI59" s="2"/>
-    </row>
-    <row r="60" spans="3:35">
+      <c r="AJ59" s="2"/>
+    </row>
+    <row r="60" spans="3:36">
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
@@ -2885,8 +2949,9 @@
       <c r="AG60" s="2"/>
       <c r="AH60" s="2"/>
       <c r="AI60" s="2"/>
-    </row>
-    <row r="61" spans="3:35">
+      <c r="AJ60" s="2"/>
+    </row>
+    <row r="61" spans="3:36">
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
@@ -2920,8 +2985,9 @@
       <c r="AG61" s="2"/>
       <c r="AH61" s="2"/>
       <c r="AI61" s="2"/>
-    </row>
-    <row r="62" spans="3:35">
+      <c r="AJ61" s="2"/>
+    </row>
+    <row r="62" spans="3:36">
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
@@ -2955,8 +3021,9 @@
       <c r="AG62" s="2"/>
       <c r="AH62" s="2"/>
       <c r="AI62" s="2"/>
-    </row>
-    <row r="63" spans="3:35">
+      <c r="AJ62" s="2"/>
+    </row>
+    <row r="63" spans="3:36">
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
@@ -2990,8 +3057,9 @@
       <c r="AG63" s="2"/>
       <c r="AH63" s="2"/>
       <c r="AI63" s="2"/>
-    </row>
-    <row r="64" spans="3:35">
+      <c r="AJ63" s="2"/>
+    </row>
+    <row r="64" spans="3:36">
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
@@ -3025,8 +3093,9 @@
       <c r="AG64" s="2"/>
       <c r="AH64" s="2"/>
       <c r="AI64" s="2"/>
-    </row>
-    <row r="65" spans="3:35">
+      <c r="AJ64" s="2"/>
+    </row>
+    <row r="65" spans="3:36">
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
@@ -3060,8 +3129,9 @@
       <c r="AG65" s="2"/>
       <c r="AH65" s="2"/>
       <c r="AI65" s="2"/>
-    </row>
-    <row r="66" spans="3:35">
+      <c r="AJ65" s="2"/>
+    </row>
+    <row r="66" spans="3:36">
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
@@ -3095,24 +3165,25 @@
       <c r="AG66" s="2"/>
       <c r="AH66" s="2"/>
       <c r="AI66" s="2"/>
+      <c r="AJ66" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B29:M29"/>
+    <mergeCell ref="B29:N29"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:I27 M2:M27" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:J27 N2:N27" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>YesNo</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J27" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K27" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>Priority</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K27" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L27" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>Status</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B29:M29" r:id="rId1" display="CLICK HERE TO CREATE IN SMARTSHEET" xr:uid="{764433F6-446C-4FC9-8A69-5DDE1CDC2C41}"/>
+    <hyperlink ref="B29:N29" r:id="rId1" display="CLICK HERE TO CREATE IN SMARTSHEET" xr:uid="{764433F6-446C-4FC9-8A69-5DDE1CDC2C41}"/>
   </hyperlinks>
   <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
   <pageSetup scale="58" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>

</xml_diff>